<commit_message>
Nuevas ventanas de color
</commit_message>
<xml_diff>
--- a/Data/Temp/Delegaciones.xlsx
+++ b/Data/Temp/Delegaciones.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ivan\Desktop\GIT_SAT\SIMETRIA\SIMETRIA_ExtraccionFreematica\Data\Temp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1079DCCE-573B-45D9-A4D9-570D84D38CC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{424D289E-671D-48D5-BD01-E4F7E48223E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-3900" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-1020" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Delegaciones" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Código</t>
   </si>
@@ -33,7 +33,34 @@
     <t>Nombre</t>
   </si>
   <si>
-    <t>CASTELLON</t>
+    <t>Abreviatura</t>
+  </si>
+  <si>
+    <t>CAS</t>
+  </si>
+  <si>
+    <t>Valencia</t>
+  </si>
+  <si>
+    <t>Castellón</t>
+  </si>
+  <si>
+    <t>VAL</t>
+  </si>
+  <si>
+    <t>Barcelona</t>
+  </si>
+  <si>
+    <t>08</t>
+  </si>
+  <si>
+    <t>BAR</t>
+  </si>
+  <si>
+    <t>Madrid</t>
+  </si>
+  <si>
+    <t>MAD</t>
   </si>
 </sst>
 </file>
@@ -69,8 +96,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -351,31 +379,76 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="3" width="9.140625" style="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
         <v>12</v>
       </c>
-      <c r="B2" t="s">
-        <v>2</v>
+      <c r="B2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>46</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>28</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError sqref="A4" numberStoredAsText="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>